<commit_message>
manual calculations for aapl
</commit_message>
<xml_diff>
--- a/input/Financial Statement AAPL/Compiled Income Statement-AAPL.xlsx
+++ b/input/Financial Statement AAPL/Compiled Income Statement-AAPL.xlsx
@@ -2273,7 +2273,9 @@
       <c r="I24" t="n">
         <v>0.73</v>
       </c>
-      <c r="J24" t="inlineStr"/>
+      <c r="J24" t="n">
+        <v>-0.73</v>
+      </c>
       <c r="K24" t="inlineStr"/>
       <c r="L24" t="inlineStr"/>
       <c r="M24" t="inlineStr"/>
@@ -4764,7 +4766,9 @@
       <c r="J21" t="n">
         <v>0.73</v>
       </c>
-      <c r="K21" t="inlineStr"/>
+      <c r="K21" t="n">
+        <v>-0.73</v>
+      </c>
       <c r="L21" t="inlineStr"/>
       <c r="M21" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
more manual calculations and documentation
</commit_message>
<xml_diff>
--- a/input/Financial Statement AAPL/Compiled Income Statement-AAPL.xlsx
+++ b/input/Financial Statement AAPL/Compiled Income Statement-AAPL.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC28"/>
+  <dimension ref="A1:AD28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,140 +442,145 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Year Ended 2016</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Q1 2017</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Q2 2017</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Q3 2017</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Q4 2017</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Year Ended 2017</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Q1 2018</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Q2 2018</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Q3 2018</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Q4 2018</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Year Ended 2018</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Q1 2019</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Q2 2019</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Q3 2019</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Q4 2019</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Year Ended 2019</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Q1 2020</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Q2 2020</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Q3 2020</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Q4 2020</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Year Ended 2020</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Q1 2021</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>Q2 2021</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>Q3 2021</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>Q4 2021</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>Year Ended 2021</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>Q1 2022</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>Q2 2022</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>Q3 2022</t>
         </is>
@@ -584,7 +589,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>income statement [abstract]</t>
+          <t>Income statement [abstract]</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -615,284 +620,294 @@
       <c r="AA2" t="inlineStr"/>
       <c r="AB2" t="inlineStr"/>
       <c r="AC2" t="inlineStr"/>
+      <c r="AD2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>net sales</t>
+          <t>Net sales</t>
         </is>
       </c>
       <c r="B3" t="n">
+        <v>215639</v>
+      </c>
+      <c r="C3" t="n">
         <v>78351</v>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>52896</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>45408</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>183826</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>229234</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>88293</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>61137</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>53265</v>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>212330</v>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
         <v>265595</v>
       </c>
-      <c r="L3" t="n">
+      <c r="M3" t="n">
         <v>84310</v>
       </c>
-      <c r="M3" t="n">
+      <c r="N3" t="n">
         <v>58015</v>
       </c>
-      <c r="N3" t="n">
+      <c r="O3" t="n">
         <v>53809</v>
       </c>
-      <c r="O3" t="n">
+      <c r="P3" t="n">
         <v>206365</v>
       </c>
-      <c r="P3" t="n">
+      <c r="Q3" t="n">
         <v>260174</v>
       </c>
-      <c r="Q3" t="n">
+      <c r="R3" t="n">
         <v>91819</v>
       </c>
-      <c r="R3" t="n">
+      <c r="S3" t="n">
         <v>58313</v>
       </c>
-      <c r="S3" t="n">
+      <c r="T3" t="n">
         <v>59685</v>
       </c>
-      <c r="T3" t="n">
+      <c r="U3" t="n">
         <v>214830</v>
       </c>
-      <c r="U3" t="n">
+      <c r="V3" t="n">
         <v>274515</v>
       </c>
-      <c r="V3" t="n">
+      <c r="W3" t="n">
         <v>111439</v>
       </c>
-      <c r="W3" t="n">
+      <c r="X3" t="n">
         <v>89584</v>
       </c>
-      <c r="X3" t="n">
+      <c r="Y3" t="n">
         <v>81434</v>
       </c>
-      <c r="Y3" t="n">
+      <c r="Z3" t="n">
         <v>284383</v>
       </c>
-      <c r="Z3" t="n">
+      <c r="AA3" t="n">
         <v>365817</v>
       </c>
-      <c r="AA3" t="n">
+      <c r="AB3" t="n">
         <v>123945</v>
       </c>
-      <c r="AB3" t="n">
+      <c r="AC3" t="n">
         <v>97278</v>
       </c>
-      <c r="AC3" t="n">
+      <c r="AD3" t="n">
         <v>82959</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>cost of sales</t>
+          <t>Cost of sales</t>
         </is>
       </c>
       <c r="B4" t="n">
+        <v>131376</v>
+      </c>
+      <c r="C4" t="n">
         <v>48175</v>
       </c>
-      <c r="C4" t="n">
+      <c r="D4" t="n">
         <v>32305</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>27920</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>113128</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>141048</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>54381</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>37715</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>32844</v>
       </c>
-      <c r="J4" t="n">
+      <c r="K4" t="n">
         <v>130912</v>
       </c>
-      <c r="K4" t="n">
+      <c r="L4" t="n">
         <v>163756</v>
       </c>
-      <c r="L4" t="n">
+      <c r="M4" t="n">
         <v>52279</v>
       </c>
-      <c r="M4" t="n">
+      <c r="N4" t="n">
         <v>36194</v>
       </c>
-      <c r="N4" t="n">
+      <c r="O4" t="n">
         <v>33582</v>
       </c>
-      <c r="O4" t="n">
+      <c r="P4" t="n">
         <v>128200</v>
       </c>
-      <c r="P4" t="n">
+      <c r="Q4" t="n">
         <v>161782</v>
       </c>
-      <c r="Q4" t="n">
+      <c r="R4" t="n">
         <v>56602</v>
       </c>
-      <c r="R4" t="n">
+      <c r="S4" t="n">
         <v>35943</v>
       </c>
-      <c r="S4" t="n">
+      <c r="T4" t="n">
         <v>37005</v>
       </c>
-      <c r="T4" t="n">
+      <c r="U4" t="n">
         <v>132554</v>
       </c>
-      <c r="U4" t="n">
+      <c r="V4" t="n">
         <v>169559</v>
       </c>
-      <c r="V4" t="n">
+      <c r="W4" t="n">
         <v>67111</v>
       </c>
-      <c r="W4" t="n">
+      <c r="X4" t="n">
         <v>51505</v>
       </c>
-      <c r="X4" t="n">
+      <c r="Y4" t="n">
         <v>46179</v>
       </c>
-      <c r="Y4" t="n">
+      <c r="Z4" t="n">
         <v>166802</v>
       </c>
-      <c r="Z4" t="n">
+      <c r="AA4" t="n">
         <v>212981</v>
       </c>
-      <c r="AA4" t="n">
+      <c r="AB4" t="n">
         <v>69702</v>
       </c>
-      <c r="AB4" t="n">
+      <c r="AC4" t="n">
         <v>54719</v>
       </c>
-      <c r="AC4" t="n">
+      <c r="AD4" t="n">
         <v>47074</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>gross margin</t>
+          <t>Gross margin</t>
         </is>
       </c>
       <c r="B5" t="n">
+        <v>84263</v>
+      </c>
+      <c r="C5" t="n">
         <v>30176</v>
       </c>
-      <c r="C5" t="n">
+      <c r="D5" t="n">
         <v>20591</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>17488</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>70698</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>88186</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>33912</v>
       </c>
-      <c r="H5" t="n">
+      <c r="I5" t="n">
         <v>23422</v>
       </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
         <v>20421</v>
       </c>
-      <c r="J5" t="n">
+      <c r="K5" t="n">
         <v>81418</v>
       </c>
-      <c r="K5" t="n">
+      <c r="L5" t="n">
         <v>101839</v>
       </c>
-      <c r="L5" t="n">
+      <c r="M5" t="n">
         <v>32031</v>
       </c>
-      <c r="M5" t="n">
+      <c r="N5" t="n">
         <v>21821</v>
       </c>
-      <c r="N5" t="n">
+      <c r="O5" t="n">
         <v>20227</v>
       </c>
-      <c r="O5" t="n">
+      <c r="P5" t="n">
         <v>78165</v>
       </c>
-      <c r="P5" t="n">
+      <c r="Q5" t="n">
         <v>98392</v>
       </c>
-      <c r="Q5" t="n">
+      <c r="R5" t="n">
         <v>35217</v>
       </c>
-      <c r="R5" t="n">
+      <c r="S5" t="n">
         <v>22370</v>
       </c>
-      <c r="S5" t="n">
+      <c r="T5" t="n">
         <v>22680</v>
       </c>
-      <c r="T5" t="n">
+      <c r="U5" t="n">
         <v>82276</v>
       </c>
-      <c r="U5" t="n">
+      <c r="V5" t="n">
         <v>104956</v>
       </c>
-      <c r="V5" t="n">
+      <c r="W5" t="n">
         <v>44328</v>
       </c>
-      <c r="W5" t="n">
+      <c r="X5" t="n">
         <v>38079</v>
       </c>
-      <c r="X5" t="n">
+      <c r="Y5" t="n">
         <v>35255</v>
       </c>
-      <c r="Y5" t="n">
+      <c r="Z5" t="n">
         <v>117581</v>
       </c>
-      <c r="Z5" t="n">
+      <c r="AA5" t="n">
         <v>152836</v>
       </c>
-      <c r="AA5" t="n">
+      <c r="AB5" t="n">
         <v>54243</v>
       </c>
-      <c r="AB5" t="n">
+      <c r="AC5" t="n">
         <v>42559</v>
       </c>
-      <c r="AC5" t="n">
+      <c r="AD5" t="n">
         <v>35885</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>operating expenses:</t>
+          <t>Operating expenses:</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
@@ -922,7 +937,8 @@
       <c r="Z6" t="inlineStr"/>
       <c r="AA6" t="inlineStr"/>
       <c r="AB6" t="inlineStr"/>
-      <c r="AC6" t="inlineStr">
+      <c r="AC6" t="inlineStr"/>
+      <c r="AD6" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -931,735 +947,759 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>research and development</t>
+          <t>Research and development</t>
         </is>
       </c>
       <c r="B7" t="n">
+        <v>10045</v>
+      </c>
+      <c r="C7" t="n">
         <v>2871</v>
       </c>
-      <c r="C7" t="n">
+      <c r="D7" t="n">
         <v>2776</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>2937</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>8644</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>11581</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>3407</v>
       </c>
-      <c r="H7" t="n">
+      <c r="I7" t="n">
         <v>3378</v>
       </c>
-      <c r="I7" t="n">
+      <c r="J7" t="n">
         <v>3701</v>
       </c>
-      <c r="J7" t="n">
+      <c r="K7" t="n">
         <v>10535</v>
       </c>
-      <c r="K7" t="n">
+      <c r="L7" t="n">
         <v>14236</v>
       </c>
-      <c r="L7" t="n">
+      <c r="M7" t="n">
         <v>3902</v>
       </c>
-      <c r="M7" t="n">
+      <c r="N7" t="n">
         <v>3948</v>
       </c>
-      <c r="N7" t="n">
+      <c r="O7" t="n">
         <v>4257</v>
       </c>
-      <c r="O7" t="n">
+      <c r="P7" t="n">
         <v>11960</v>
       </c>
-      <c r="P7" t="n">
+      <c r="Q7" t="n">
         <v>16217</v>
       </c>
-      <c r="Q7" t="n">
+      <c r="R7" t="n">
         <v>4451</v>
       </c>
-      <c r="R7" t="n">
+      <c r="S7" t="n">
         <v>4565</v>
       </c>
-      <c r="S7" t="n">
+      <c r="T7" t="n">
         <v>4758</v>
       </c>
-      <c r="T7" t="n">
+      <c r="U7" t="n">
         <v>13994</v>
       </c>
-      <c r="U7" t="n">
+      <c r="V7" t="n">
         <v>18752</v>
       </c>
-      <c r="V7" t="n">
+      <c r="W7" t="n">
         <v>5163</v>
       </c>
-      <c r="W7" t="n">
+      <c r="X7" t="n">
         <v>5262</v>
       </c>
-      <c r="X7" t="n">
+      <c r="Y7" t="n">
         <v>5717</v>
       </c>
-      <c r="Y7" t="n">
+      <c r="Z7" t="n">
         <v>16197</v>
       </c>
-      <c r="Z7" t="n">
+      <c r="AA7" t="n">
         <v>21914</v>
       </c>
-      <c r="AA7" t="n">
+      <c r="AB7" t="n">
         <v>6306</v>
       </c>
-      <c r="AB7" t="n">
+      <c r="AC7" t="n">
         <v>6387</v>
       </c>
-      <c r="AC7" t="n">
+      <c r="AD7" t="n">
         <v>6797</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>selling, general and administrative</t>
+          <t>Selling, general and administrative</t>
         </is>
       </c>
       <c r="B8" t="n">
+        <v>14194</v>
+      </c>
+      <c r="C8" t="n">
         <v>3946</v>
       </c>
-      <c r="C8" t="n">
+      <c r="D8" t="n">
         <v>3718</v>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
         <v>3783</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>11478</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>15261</v>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>4231</v>
       </c>
-      <c r="H8" t="n">
+      <c r="I8" t="n">
         <v>4150</v>
       </c>
-      <c r="I8" t="n">
+      <c r="J8" t="n">
         <v>4108</v>
       </c>
-      <c r="J8" t="n">
+      <c r="K8" t="n">
         <v>12597</v>
       </c>
-      <c r="K8" t="n">
+      <c r="L8" t="n">
         <v>16705</v>
       </c>
-      <c r="L8" t="n">
+      <c r="M8" t="n">
         <v>4783</v>
       </c>
-      <c r="M8" t="n">
+      <c r="N8" t="n">
         <v>4458</v>
       </c>
-      <c r="N8" t="n">
+      <c r="O8" t="n">
         <v>4426</v>
       </c>
-      <c r="O8" t="n">
+      <c r="P8" t="n">
         <v>13819</v>
       </c>
-      <c r="P8" t="n">
+      <c r="Q8" t="n">
         <v>18245</v>
       </c>
-      <c r="Q8" t="n">
+      <c r="R8" t="n">
         <v>5197</v>
       </c>
-      <c r="R8" t="n">
+      <c r="S8" t="n">
         <v>4952</v>
       </c>
-      <c r="S8" t="n">
+      <c r="T8" t="n">
         <v>4831</v>
       </c>
-      <c r="T8" t="n">
+      <c r="U8" t="n">
         <v>15085</v>
       </c>
-      <c r="U8" t="n">
+      <c r="V8" t="n">
         <v>19916</v>
       </c>
-      <c r="V8" t="n">
+      <c r="W8" t="n">
         <v>5631</v>
       </c>
-      <c r="W8" t="n">
+      <c r="X8" t="n">
         <v>5314</v>
       </c>
-      <c r="X8" t="n">
+      <c r="Y8" t="n">
         <v>5412</v>
       </c>
-      <c r="Y8" t="n">
+      <c r="Z8" t="n">
         <v>16561</v>
       </c>
-      <c r="Z8" t="n">
+      <c r="AA8" t="n">
         <v>21973</v>
       </c>
-      <c r="AA8" t="n">
+      <c r="AB8" t="n">
         <v>6449</v>
       </c>
-      <c r="AB8" t="n">
+      <c r="AC8" t="n">
         <v>6193</v>
       </c>
-      <c r="AC8" t="n">
+      <c r="AD8" t="n">
         <v>6012</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>total operating expenses</t>
+          <t>Total operating expenses</t>
         </is>
       </c>
       <c r="B9" t="n">
+        <v>24239</v>
+      </c>
+      <c r="C9" t="n">
         <v>6817</v>
       </c>
-      <c r="C9" t="n">
+      <c r="D9" t="n">
         <v>6494</v>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
         <v>6720</v>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>20122</v>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
         <v>26842</v>
       </c>
-      <c r="G9" t="n">
+      <c r="H9" t="n">
         <v>7638</v>
       </c>
-      <c r="H9" t="n">
+      <c r="I9" t="n">
         <v>7528</v>
       </c>
-      <c r="I9" t="n">
+      <c r="J9" t="n">
         <v>7809</v>
       </c>
-      <c r="J9" t="n">
+      <c r="K9" t="n">
         <v>23132</v>
       </c>
-      <c r="K9" t="n">
+      <c r="L9" t="n">
         <v>30941</v>
       </c>
-      <c r="L9" t="n">
+      <c r="M9" t="n">
         <v>8685</v>
       </c>
-      <c r="M9" t="n">
+      <c r="N9" t="n">
         <v>8406</v>
       </c>
-      <c r="N9" t="n">
+      <c r="O9" t="n">
         <v>8683</v>
       </c>
-      <c r="O9" t="n">
+      <c r="P9" t="n">
         <v>25779</v>
       </c>
-      <c r="P9" t="n">
+      <c r="Q9" t="n">
         <v>34462</v>
       </c>
-      <c r="Q9" t="n">
+      <c r="R9" t="n">
         <v>9648</v>
       </c>
-      <c r="R9" t="n">
+      <c r="S9" t="n">
         <v>9517</v>
       </c>
-      <c r="S9" t="n">
+      <c r="T9" t="n">
         <v>9589</v>
       </c>
-      <c r="T9" t="n">
+      <c r="U9" t="n">
         <v>29079</v>
       </c>
-      <c r="U9" t="n">
+      <c r="V9" t="n">
         <v>38668</v>
       </c>
-      <c r="V9" t="n">
+      <c r="W9" t="n">
         <v>10794</v>
       </c>
-      <c r="W9" t="n">
+      <c r="X9" t="n">
         <v>10576</v>
       </c>
-      <c r="X9" t="n">
+      <c r="Y9" t="n">
         <v>11129</v>
       </c>
-      <c r="Y9" t="n">
+      <c r="Z9" t="n">
         <v>32758</v>
       </c>
-      <c r="Z9" t="n">
+      <c r="AA9" t="n">
         <v>43887</v>
       </c>
-      <c r="AA9" t="n">
+      <c r="AB9" t="n">
         <v>12755</v>
       </c>
-      <c r="AB9" t="n">
+      <c r="AC9" t="n">
         <v>12580</v>
       </c>
-      <c r="AC9" t="n">
+      <c r="AD9" t="n">
         <v>12809</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>operating income</t>
+          <t>Operating income</t>
         </is>
       </c>
       <c r="B10" t="n">
+        <v>60024</v>
+      </c>
+      <c r="C10" t="n">
         <v>23359</v>
       </c>
-      <c r="C10" t="n">
+      <c r="D10" t="n">
         <v>14097</v>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
         <v>10768</v>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
         <v>50576</v>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
         <v>61344</v>
       </c>
-      <c r="G10" t="n">
+      <c r="H10" t="n">
         <v>26274</v>
       </c>
-      <c r="H10" t="n">
+      <c r="I10" t="n">
         <v>15894</v>
       </c>
-      <c r="I10" t="n">
+      <c r="J10" t="n">
         <v>12612</v>
       </c>
-      <c r="J10" t="n">
+      <c r="K10" t="n">
         <v>58286</v>
       </c>
-      <c r="K10" t="n">
+      <c r="L10" t="n">
         <v>70898</v>
       </c>
-      <c r="L10" t="n">
+      <c r="M10" t="n">
         <v>23346</v>
       </c>
-      <c r="M10" t="n">
+      <c r="N10" t="n">
         <v>13415</v>
       </c>
-      <c r="N10" t="n">
+      <c r="O10" t="n">
         <v>11544</v>
       </c>
-      <c r="O10" t="n">
+      <c r="P10" t="n">
         <v>52386</v>
       </c>
-      <c r="P10" t="n">
+      <c r="Q10" t="n">
         <v>63930</v>
       </c>
-      <c r="Q10" t="n">
+      <c r="R10" t="n">
         <v>25569</v>
       </c>
-      <c r="R10" t="n">
+      <c r="S10" t="n">
         <v>12853</v>
       </c>
-      <c r="S10" t="n">
+      <c r="T10" t="n">
         <v>13091</v>
       </c>
-      <c r="T10" t="n">
+      <c r="U10" t="n">
         <v>53197</v>
       </c>
-      <c r="U10" t="n">
+      <c r="V10" t="n">
         <v>66288</v>
       </c>
-      <c r="V10" t="n">
+      <c r="W10" t="n">
         <v>33534</v>
       </c>
-      <c r="W10" t="n">
+      <c r="X10" t="n">
         <v>27503</v>
       </c>
-      <c r="X10" t="n">
+      <c r="Y10" t="n">
         <v>24126</v>
       </c>
-      <c r="Y10" t="n">
+      <c r="Z10" t="n">
         <v>84823</v>
       </c>
-      <c r="Z10" t="n">
+      <c r="AA10" t="n">
         <v>108949</v>
       </c>
-      <c r="AA10" t="n">
+      <c r="AB10" t="n">
         <v>41488</v>
       </c>
-      <c r="AB10" t="n">
+      <c r="AC10" t="n">
         <v>29979</v>
       </c>
-      <c r="AC10" t="n">
+      <c r="AD10" t="n">
         <v>23076</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>other income, net</t>
+          <t>Other income/, net</t>
         </is>
       </c>
       <c r="B11" t="n">
+        <v>1348</v>
+      </c>
+      <c r="C11" t="n">
         <v>821</v>
       </c>
-      <c r="C11" t="n">
+      <c r="D11" t="n">
         <v>587</v>
       </c>
-      <c r="D11" t="n">
+      <c r="E11" t="n">
         <v>540</v>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
         <v>2205</v>
       </c>
-      <c r="F11" t="n">
+      <c r="G11" t="n">
         <v>2745</v>
       </c>
-      <c r="G11" t="n">
+      <c r="H11" t="n">
         <v>756</v>
       </c>
-      <c r="H11" t="n">
+      <c r="I11" t="n">
         <v>274</v>
       </c>
-      <c r="I11" t="n">
+      <c r="J11" t="n">
         <v>672</v>
       </c>
-      <c r="J11" t="n">
+      <c r="K11" t="n">
         <v>1333</v>
       </c>
-      <c r="K11" t="n">
+      <c r="L11" t="n">
         <v>2005</v>
       </c>
-      <c r="L11" t="n">
+      <c r="M11" t="n">
         <v>560</v>
       </c>
-      <c r="M11" t="n">
+      <c r="N11" t="n">
         <v>378</v>
       </c>
-      <c r="N11" t="n">
+      <c r="O11" t="n">
         <v>367</v>
       </c>
-      <c r="O11" t="n">
+      <c r="P11" t="n">
         <v>1440</v>
       </c>
-      <c r="P11" t="n">
+      <c r="Q11" t="n">
         <v>1807</v>
       </c>
-      <c r="Q11" t="n">
+      <c r="R11" t="n">
         <v>349</v>
       </c>
-      <c r="R11" t="n">
+      <c r="S11" t="n">
         <v>282</v>
       </c>
-      <c r="S11" t="n">
+      <c r="T11" t="n">
         <v>46</v>
       </c>
-      <c r="T11" t="n">
+      <c r="U11" t="n">
         <v>757</v>
       </c>
-      <c r="U11" t="n">
+      <c r="V11" t="n">
         <v>803</v>
       </c>
-      <c r="V11" t="n">
+      <c r="W11" t="n">
         <v>45</v>
       </c>
-      <c r="W11" t="n">
+      <c r="X11" t="n">
         <v>508</v>
       </c>
-      <c r="X11" t="n">
+      <c r="Y11" t="n">
         <v>243</v>
       </c>
-      <c r="Y11" t="n">
+      <c r="Z11" t="n">
         <v>15</v>
       </c>
-      <c r="Z11" t="n">
+      <c r="AA11" t="n">
         <v>258</v>
       </c>
-      <c r="AA11" t="n">
+      <c r="AB11" t="n">
         <v>-247</v>
       </c>
-      <c r="AB11" t="n">
+      <c r="AC11" t="n">
         <v>160</v>
       </c>
-      <c r="AC11" t="n">
+      <c r="AD11" t="n">
         <v>-10</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>income before provision for income taxes</t>
+          <t>Income before provision for income taxes</t>
         </is>
       </c>
       <c r="B12" t="n">
+        <v>61372</v>
+      </c>
+      <c r="C12" t="n">
         <v>24180</v>
       </c>
-      <c r="C12" t="n">
+      <c r="D12" t="n">
         <v>14684</v>
       </c>
-      <c r="D12" t="n">
+      <c r="E12" t="n">
         <v>11308</v>
       </c>
-      <c r="E12" t="n">
+      <c r="F12" t="n">
         <v>52781</v>
       </c>
-      <c r="F12" t="n">
+      <c r="G12" t="n">
         <v>64089</v>
       </c>
-      <c r="G12" t="n">
+      <c r="H12" t="n">
         <v>27030</v>
       </c>
-      <c r="H12" t="n">
+      <c r="I12" t="n">
         <v>16168</v>
       </c>
-      <c r="I12" t="n">
+      <c r="J12" t="n">
         <v>13284</v>
       </c>
-      <c r="J12" t="n">
+      <c r="K12" t="n">
         <v>59619</v>
       </c>
-      <c r="K12" t="n">
+      <c r="L12" t="n">
         <v>72903</v>
       </c>
-      <c r="L12" t="n">
+      <c r="M12" t="n">
         <v>23906</v>
       </c>
-      <c r="M12" t="n">
+      <c r="N12" t="n">
         <v>13793</v>
       </c>
-      <c r="N12" t="n">
+      <c r="O12" t="n">
         <v>11911</v>
       </c>
-      <c r="O12" t="n">
+      <c r="P12" t="n">
         <v>53826</v>
       </c>
-      <c r="P12" t="n">
+      <c r="Q12" t="n">
         <v>65737</v>
       </c>
-      <c r="Q12" t="n">
+      <c r="R12" t="n">
         <v>25918</v>
       </c>
-      <c r="R12" t="n">
+      <c r="S12" t="n">
         <v>13135</v>
       </c>
-      <c r="S12" t="n">
+      <c r="T12" t="n">
         <v>13137</v>
       </c>
-      <c r="T12" t="n">
+      <c r="U12" t="n">
         <v>53954</v>
       </c>
-      <c r="U12" t="n">
+      <c r="V12" t="n">
         <v>67091</v>
       </c>
-      <c r="V12" t="n">
+      <c r="W12" t="n">
         <v>33579</v>
       </c>
-      <c r="W12" t="n">
+      <c r="X12" t="n">
         <v>28011</v>
       </c>
-      <c r="X12" t="n">
+      <c r="Y12" t="n">
         <v>24369</v>
       </c>
-      <c r="Y12" t="n">
+      <c r="Z12" t="n">
         <v>84838</v>
       </c>
-      <c r="Z12" t="n">
+      <c r="AA12" t="n">
         <v>109207</v>
       </c>
-      <c r="AA12" t="n">
+      <c r="AB12" t="n">
         <v>41241</v>
       </c>
-      <c r="AB12" t="n">
+      <c r="AC12" t="n">
         <v>30139</v>
       </c>
-      <c r="AC12" t="n">
+      <c r="AD12" t="n">
         <v>23066</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>provision for income taxes</t>
+          <t>Provision for income taxes</t>
         </is>
       </c>
       <c r="B13" t="n">
+        <v>15685</v>
+      </c>
+      <c r="C13" t="n">
         <v>6289</v>
       </c>
-      <c r="C13" t="n">
+      <c r="D13" t="n">
         <v>3655</v>
       </c>
-      <c r="D13" t="n">
+      <c r="E13" t="n">
         <v>2591</v>
       </c>
-      <c r="E13" t="n">
+      <c r="F13" t="n">
         <v>13147</v>
       </c>
-      <c r="F13" t="n">
+      <c r="G13" t="n">
         <v>15738</v>
       </c>
-      <c r="G13" t="n">
+      <c r="H13" t="n">
         <v>6965</v>
       </c>
-      <c r="H13" t="n">
+      <c r="I13" t="n">
         <v>2346</v>
       </c>
-      <c r="I13" t="n">
+      <c r="J13" t="n">
         <v>1765</v>
       </c>
-      <c r="J13" t="n">
+      <c r="K13" t="n">
         <v>11607</v>
       </c>
-      <c r="K13" t="n">
+      <c r="L13" t="n">
         <v>13372</v>
       </c>
-      <c r="L13" t="n">
+      <c r="M13" t="n">
         <v>3941</v>
       </c>
-      <c r="M13" t="n">
+      <c r="N13" t="n">
         <v>2232</v>
       </c>
-      <c r="N13" t="n">
+      <c r="O13" t="n">
         <v>1867</v>
       </c>
-      <c r="O13" t="n">
+      <c r="P13" t="n">
         <v>8614</v>
       </c>
-      <c r="P13" t="n">
+      <c r="Q13" t="n">
         <v>10481</v>
       </c>
-      <c r="Q13" t="n">
+      <c r="R13" t="n">
         <v>3682</v>
       </c>
-      <c r="R13" t="n">
+      <c r="S13" t="n">
         <v>1886</v>
       </c>
-      <c r="S13" t="n">
+      <c r="T13" t="n">
         <v>1884</v>
       </c>
-      <c r="T13" t="n">
+      <c r="U13" t="n">
         <v>7796</v>
       </c>
-      <c r="U13" t="n">
+      <c r="V13" t="n">
         <v>9680</v>
       </c>
-      <c r="V13" t="n">
+      <c r="W13" t="n">
         <v>4824</v>
       </c>
-      <c r="W13" t="n">
+      <c r="X13" t="n">
         <v>4381</v>
       </c>
-      <c r="X13" t="n">
+      <c r="Y13" t="n">
         <v>2625</v>
       </c>
-      <c r="Y13" t="n">
+      <c r="Z13" t="n">
         <v>11902</v>
       </c>
-      <c r="Z13" t="n">
+      <c r="AA13" t="n">
         <v>14527</v>
       </c>
-      <c r="AA13" t="n">
+      <c r="AB13" t="n">
         <v>6611</v>
       </c>
-      <c r="AB13" t="n">
+      <c r="AC13" t="n">
         <v>5129</v>
       </c>
-      <c r="AC13" t="n">
+      <c r="AD13" t="n">
         <v>3624</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>net income</t>
+          <t>Net income</t>
         </is>
       </c>
       <c r="B14" t="n">
+        <v>45687</v>
+      </c>
+      <c r="C14" t="n">
         <v>17891</v>
       </c>
-      <c r="C14" t="n">
+      <c r="D14" t="n">
         <v>11029</v>
       </c>
-      <c r="D14" t="n">
+      <c r="E14" t="n">
         <v>8717</v>
       </c>
-      <c r="E14" t="n">
+      <c r="F14" t="n">
         <v>39634</v>
       </c>
-      <c r="F14" t="n">
+      <c r="G14" t="n">
         <v>48351</v>
       </c>
-      <c r="G14" t="n">
+      <c r="H14" t="n">
         <v>20065</v>
       </c>
-      <c r="H14" t="n">
+      <c r="I14" t="n">
         <v>13822</v>
       </c>
-      <c r="I14" t="n">
+      <c r="J14" t="n">
         <v>11519</v>
       </c>
-      <c r="J14" t="n">
+      <c r="K14" t="n">
         <v>48012</v>
       </c>
-      <c r="K14" t="n">
+      <c r="L14" t="n">
         <v>59531</v>
       </c>
-      <c r="L14" t="n">
+      <c r="M14" t="n">
         <v>19965</v>
       </c>
-      <c r="M14" t="n">
+      <c r="N14" t="n">
         <v>11561</v>
       </c>
-      <c r="N14" t="n">
+      <c r="O14" t="n">
         <v>10044</v>
       </c>
-      <c r="O14" t="n">
+      <c r="P14" t="n">
         <v>45212</v>
       </c>
-      <c r="P14" t="n">
+      <c r="Q14" t="n">
         <v>55256</v>
       </c>
-      <c r="Q14" t="n">
+      <c r="R14" t="n">
         <v>22236</v>
       </c>
-      <c r="R14" t="n">
+      <c r="S14" t="n">
         <v>11249</v>
       </c>
-      <c r="S14" t="n">
+      <c r="T14" t="n">
         <v>11253</v>
       </c>
-      <c r="T14" t="n">
+      <c r="U14" t="n">
         <v>46158</v>
       </c>
-      <c r="U14" t="n">
+      <c r="V14" t="n">
         <v>57411</v>
       </c>
-      <c r="V14" t="n">
+      <c r="W14" t="n">
         <v>28755</v>
       </c>
-      <c r="W14" t="n">
+      <c r="X14" t="n">
         <v>23630</v>
       </c>
-      <c r="X14" t="n">
+      <c r="Y14" t="n">
         <v>21744</v>
       </c>
-      <c r="Y14" t="n">
+      <c r="Z14" t="n">
         <v>72936</v>
       </c>
-      <c r="Z14" t="n">
+      <c r="AA14" t="n">
         <v>94680</v>
       </c>
-      <c r="AA14" t="n">
+      <c r="AB14" t="n">
         <v>34630</v>
       </c>
-      <c r="AB14" t="n">
+      <c r="AC14" t="n">
         <v>25010</v>
       </c>
-      <c r="AC14" t="n">
+      <c r="AD14" t="n">
         <v>19442</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>earnings per share [abstract]</t>
+          <t>Earnings per share [abstract]</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
@@ -1690,11 +1730,12 @@
       <c r="AA15" t="inlineStr"/>
       <c r="AB15" t="inlineStr"/>
       <c r="AC15" t="inlineStr"/>
+      <c r="AD15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>earnings per share:</t>
+          <t>Earnings per share:</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
@@ -1724,7 +1765,8 @@
       <c r="Z16" t="inlineStr"/>
       <c r="AA16" t="inlineStr"/>
       <c r="AB16" t="inlineStr"/>
-      <c r="AC16" t="inlineStr">
+      <c r="AC16" t="inlineStr"/>
+      <c r="AD16" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -1733,189 +1775,195 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>basic</t>
+          <t>Basic</t>
         </is>
       </c>
       <c r="B17" t="n">
+        <v>8.35</v>
+      </c>
+      <c r="C17" t="n">
         <v>3.38</v>
       </c>
-      <c r="C17" t="n">
+      <c r="D17" t="n">
         <v>2.11</v>
       </c>
-      <c r="D17" t="n">
+      <c r="E17" t="n">
         <v>1.68</v>
       </c>
-      <c r="E17" t="n">
+      <c r="F17" t="n">
         <v>7.59</v>
       </c>
-      <c r="F17" t="n">
+      <c r="G17" t="n">
         <v>9.27</v>
       </c>
-      <c r="G17" t="n">
+      <c r="H17" t="n">
         <v>3.92</v>
       </c>
-      <c r="H17" t="n">
+      <c r="I17" t="n">
         <v>2.75</v>
       </c>
-      <c r="I17" t="n">
+      <c r="J17" t="n">
         <v>2.36</v>
       </c>
-      <c r="J17" t="n">
+      <c r="K17" t="n">
         <v>9.65</v>
       </c>
-      <c r="K17" t="n">
+      <c r="L17" t="n">
         <v>12.01</v>
       </c>
-      <c r="L17" t="n">
+      <c r="M17" t="n">
         <v>4.22</v>
       </c>
-      <c r="M17" t="n">
+      <c r="N17" t="n">
         <v>2.47</v>
       </c>
-      <c r="N17" t="n">
+      <c r="O17" t="n">
         <v>2.2</v>
       </c>
-      <c r="O17" t="n">
+      <c r="P17" t="n">
         <v>9.77</v>
       </c>
-      <c r="P17" t="n">
+      <c r="Q17" t="n">
         <v>11.97</v>
       </c>
-      <c r="Q17" t="n">
+      <c r="R17" t="n">
         <v>5.04</v>
       </c>
-      <c r="R17" t="n">
+      <c r="S17" t="n">
         <v>2.58</v>
       </c>
-      <c r="S17" t="n">
+      <c r="T17" t="n">
         <v>2.61</v>
       </c>
-      <c r="T17" t="n">
+      <c r="U17" t="n">
         <v>0.7000000000000002</v>
       </c>
-      <c r="U17" t="n">
+      <c r="V17" t="n">
         <v>3.31</v>
       </c>
-      <c r="V17" t="n">
+      <c r="W17" t="n">
         <v>1.7</v>
       </c>
-      <c r="W17" t="n">
+      <c r="X17" t="n">
         <v>1.41</v>
       </c>
-      <c r="X17" t="n">
+      <c r="Y17" t="n">
         <v>1.31</v>
       </c>
-      <c r="Y17" t="n">
+      <c r="Z17" t="n">
         <v>4.359999999999999</v>
       </c>
-      <c r="Z17" t="n">
+      <c r="AA17" t="n">
         <v>5.67</v>
       </c>
-      <c r="AA17" t="n">
+      <c r="AB17" t="n">
         <v>2.11</v>
       </c>
-      <c r="AB17" t="n">
+      <c r="AC17" t="n">
         <v>1.54</v>
       </c>
-      <c r="AC17" t="n">
+      <c r="AD17" t="n">
         <v>1.2</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>diluted</t>
+          <t>Diluted</t>
         </is>
       </c>
       <c r="B18" t="n">
+        <v>8.31</v>
+      </c>
+      <c r="C18" t="n">
         <v>3.36</v>
       </c>
-      <c r="C18" t="n">
+      <c r="D18" t="n">
         <v>2.1</v>
       </c>
-      <c r="D18" t="n">
+      <c r="E18" t="n">
         <v>1.67</v>
       </c>
-      <c r="E18" t="n">
+      <c r="F18" t="n">
         <v>7.540000000000001</v>
       </c>
-      <c r="F18" t="n">
+      <c r="G18" t="n">
         <v>9.210000000000001</v>
       </c>
-      <c r="G18" t="n">
+      <c r="H18" t="n">
         <v>3.89</v>
       </c>
-      <c r="H18" t="n">
+      <c r="I18" t="n">
         <v>2.73</v>
       </c>
-      <c r="I18" t="n">
+      <c r="J18" t="n">
         <v>2.34</v>
       </c>
-      <c r="J18" t="n">
+      <c r="K18" t="n">
         <v>9.57</v>
       </c>
-      <c r="K18" t="n">
+      <c r="L18" t="n">
         <v>11.91</v>
       </c>
-      <c r="L18" t="n">
+      <c r="M18" t="n">
         <v>4.18</v>
       </c>
-      <c r="M18" t="n">
+      <c r="N18" t="n">
         <v>2.46</v>
       </c>
-      <c r="N18" t="n">
+      <c r="O18" t="n">
         <v>2.18</v>
       </c>
-      <c r="O18" t="n">
+      <c r="P18" t="n">
         <v>9.710000000000001</v>
       </c>
-      <c r="P18" t="n">
+      <c r="Q18" t="n">
         <v>11.89</v>
       </c>
-      <c r="Q18" t="n">
+      <c r="R18" t="n">
         <v>4.99</v>
       </c>
-      <c r="R18" t="n">
+      <c r="S18" t="n">
         <v>2.55</v>
       </c>
-      <c r="S18" t="n">
+      <c r="T18" t="n">
         <v>2.58</v>
       </c>
-      <c r="T18" t="n">
+      <c r="U18" t="n">
         <v>0.6999999999999997</v>
       </c>
-      <c r="U18" t="n">
+      <c r="V18" t="n">
         <v>3.28</v>
       </c>
-      <c r="V18" t="n">
+      <c r="W18" t="n">
         <v>1.68</v>
       </c>
-      <c r="W18" t="n">
+      <c r="X18" t="n">
         <v>1.4</v>
       </c>
-      <c r="X18" t="n">
+      <c r="Y18" t="n">
         <v>1.3</v>
       </c>
-      <c r="Y18" t="n">
+      <c r="Z18" t="n">
         <v>4.31</v>
       </c>
-      <c r="Z18" t="n">
+      <c r="AA18" t="n">
         <v>5.61</v>
       </c>
-      <c r="AA18" t="n">
+      <c r="AB18" t="n">
         <v>2.1</v>
       </c>
-      <c r="AB18" t="n">
+      <c r="AC18" t="n">
         <v>1.52</v>
       </c>
-      <c r="AC18" t="n">
+      <c r="AD18" t="n">
         <v>1.2</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>shares used in computing earnings per share:</t>
+          <t>Shares used in computing earnings per share:</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
@@ -1945,7 +1993,8 @@
       <c r="Z19" t="inlineStr"/>
       <c r="AA19" t="inlineStr"/>
       <c r="AB19" t="inlineStr"/>
-      <c r="AC19" t="inlineStr">
+      <c r="AC19" t="inlineStr"/>
+      <c r="AD19" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -1954,189 +2003,195 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>basic</t>
+          <t>Basic</t>
         </is>
       </c>
       <c r="B20" t="n">
+        <v>5470820</v>
+      </c>
+      <c r="C20" t="n">
         <v>5298661</v>
       </c>
-      <c r="C20" t="n">
+      <c r="D20" t="n">
         <v>5225791</v>
       </c>
-      <c r="D20" t="n">
+      <c r="E20" t="n">
         <v>5195088</v>
       </c>
-      <c r="E20" t="n">
+      <c r="F20" t="n">
         <v>22154</v>
       </c>
-      <c r="F20" t="n">
+      <c r="G20" t="n">
         <v>5217242</v>
       </c>
-      <c r="G20" t="n">
+      <c r="H20" t="n">
         <v>5112877</v>
       </c>
-      <c r="H20" t="n">
+      <c r="I20" t="n">
         <v>5024877</v>
       </c>
-      <c r="I20" t="n">
+      <c r="J20" t="n">
         <v>4882167</v>
       </c>
-      <c r="J20" t="n">
+      <c r="K20" t="n">
         <v>73210</v>
       </c>
-      <c r="K20" t="n">
+      <c r="L20" t="n">
         <v>4955377</v>
       </c>
-      <c r="L20" t="n">
+      <c r="M20" t="n">
         <v>4735820</v>
       </c>
-      <c r="M20" t="n">
+      <c r="N20" t="n">
         <v>4674071</v>
       </c>
-      <c r="N20" t="n">
+      <c r="O20" t="n">
         <v>4570633</v>
       </c>
-      <c r="O20" t="n">
+      <c r="P20" t="n">
         <v>47201</v>
       </c>
-      <c r="P20" t="n">
+      <c r="Q20" t="n">
         <v>4617834</v>
       </c>
-      <c r="Q20" t="n">
+      <c r="R20" t="n">
         <v>4415040</v>
       </c>
-      <c r="R20" t="n">
+      <c r="S20" t="n">
         <v>4360101</v>
       </c>
-      <c r="S20" t="n">
+      <c r="T20" t="n">
         <v>4312573</v>
       </c>
-      <c r="T20" t="n">
+      <c r="U20" t="n">
         <v>13039546</v>
       </c>
-      <c r="U20" t="n">
+      <c r="V20" t="n">
         <v>17352119</v>
       </c>
-      <c r="V20" t="n">
+      <c r="W20" t="n">
         <v>16935119</v>
       </c>
-      <c r="W20" t="n">
+      <c r="X20" t="n">
         <v>16753476</v>
       </c>
-      <c r="X20" t="n">
+      <c r="Y20" t="n">
         <v>16629371</v>
       </c>
-      <c r="Y20" t="n">
+      <c r="Z20" t="n">
         <v>71901</v>
       </c>
-      <c r="Z20" t="n">
+      <c r="AA20" t="n">
         <v>16701272</v>
       </c>
-      <c r="AA20" t="n">
+      <c r="AB20" t="n">
         <v>16391724</v>
       </c>
-      <c r="AB20" t="n">
+      <c r="AC20" t="n">
         <v>16278802</v>
       </c>
-      <c r="AC20" t="n">
+      <c r="AD20" t="n">
         <v>16162945</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>diluted</t>
+          <t>Diluted</t>
         </is>
       </c>
       <c r="B21" t="n">
+        <v>5500281</v>
+      </c>
+      <c r="C21" t="n">
         <v>5327995</v>
       </c>
-      <c r="C21" t="n">
+      <c r="D21" t="n">
         <v>5261688</v>
       </c>
-      <c r="D21" t="n">
+      <c r="E21" t="n">
         <v>5233499</v>
       </c>
-      <c r="E21" t="n">
+      <c r="F21" t="n">
         <v>18193</v>
       </c>
-      <c r="F21" t="n">
+      <c r="G21" t="n">
         <v>5251692</v>
       </c>
-      <c r="G21" t="n">
+      <c r="H21" t="n">
         <v>5157787</v>
       </c>
-      <c r="H21" t="n">
+      <c r="I21" t="n">
         <v>5068493</v>
       </c>
-      <c r="I21" t="n">
+      <c r="J21" t="n">
         <v>4926609</v>
       </c>
-      <c r="J21" t="n">
+      <c r="K21" t="n">
         <v>73500</v>
       </c>
-      <c r="K21" t="n">
+      <c r="L21" t="n">
         <v>5000109</v>
       </c>
-      <c r="L21" t="n">
+      <c r="M21" t="n">
         <v>4773252</v>
       </c>
-      <c r="M21" t="n">
+      <c r="N21" t="n">
         <v>4700646</v>
       </c>
-      <c r="N21" t="n">
+      <c r="O21" t="n">
         <v>4601380</v>
       </c>
-      <c r="O21" t="n">
+      <c r="P21" t="n">
         <v>47533</v>
       </c>
-      <c r="P21" t="n">
+      <c r="Q21" t="n">
         <v>4648913</v>
       </c>
-      <c r="Q21" t="n">
+      <c r="R21" t="n">
         <v>4454604</v>
       </c>
-      <c r="R21" t="n">
+      <c r="S21" t="n">
         <v>4404691</v>
       </c>
-      <c r="S21" t="n">
+      <c r="T21" t="n">
         <v>4354788</v>
       </c>
-      <c r="T21" t="n">
+      <c r="U21" t="n">
         <v>13173426</v>
       </c>
-      <c r="U21" t="n">
+      <c r="V21" t="n">
         <v>17528214</v>
       </c>
-      <c r="V21" t="n">
+      <c r="W21" t="n">
         <v>17113688</v>
       </c>
-      <c r="W21" t="n">
+      <c r="X21" t="n">
         <v>16929157</v>
       </c>
-      <c r="X21" t="n">
+      <c r="Y21" t="n">
         <v>16781735</v>
       </c>
-      <c r="Y21" t="n">
+      <c r="Z21" t="n">
         <v>83184</v>
       </c>
-      <c r="Z21" t="n">
+      <c r="AA21" t="n">
         <v>16864919</v>
       </c>
-      <c r="AA21" t="n">
+      <c r="AB21" t="n">
         <v>16519291</v>
       </c>
-      <c r="AB21" t="n">
+      <c r="AC21" t="n">
         <v>16403316</v>
       </c>
-      <c r="AC21" t="n">
+      <c r="AD21" t="n">
         <v>16262203</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>products</t>
+          <t>Products</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
@@ -2166,7 +2221,8 @@
       <c r="Z22" t="inlineStr"/>
       <c r="AA22" t="inlineStr"/>
       <c r="AB22" t="inlineStr"/>
-      <c r="AC22" t="inlineStr">
+      <c r="AC22" t="inlineStr"/>
+      <c r="AD22" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -2175,7 +2231,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>net sales</t>
+          <t>Net sales</t>
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
@@ -2188,95 +2244,98 @@
       <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr"/>
       <c r="K23" t="inlineStr"/>
-      <c r="L23" t="n">
+      <c r="L23" t="inlineStr"/>
+      <c r="M23" t="n">
         <v>73435</v>
       </c>
-      <c r="M23" t="n">
+      <c r="N23" t="n">
         <v>46565</v>
       </c>
-      <c r="N23" t="n">
+      <c r="O23" t="n">
         <v>42354</v>
       </c>
-      <c r="O23" t="n">
+      <c r="P23" t="n">
         <v>171529</v>
       </c>
-      <c r="P23" t="n">
+      <c r="Q23" t="n">
         <v>213883</v>
       </c>
-      <c r="Q23" t="n">
+      <c r="R23" t="n">
         <v>79104</v>
       </c>
-      <c r="R23" t="n">
+      <c r="S23" t="n">
         <v>44965</v>
       </c>
-      <c r="S23" t="n">
+      <c r="T23" t="n">
         <v>46529</v>
       </c>
-      <c r="T23" t="n">
+      <c r="U23" t="n">
         <v>174218</v>
       </c>
-      <c r="U23" t="n">
+      <c r="V23" t="n">
         <v>220747</v>
       </c>
-      <c r="V23" t="n">
+      <c r="W23" t="n">
         <v>95678</v>
       </c>
-      <c r="W23" t="n">
+      <c r="X23" t="n">
         <v>72683</v>
       </c>
-      <c r="X23" t="n">
+      <c r="Y23" t="n">
         <v>63948</v>
       </c>
-      <c r="Y23" t="n">
+      <c r="Z23" t="n">
         <v>233444</v>
       </c>
-      <c r="Z23" t="n">
+      <c r="AA23" t="n">
         <v>297392</v>
       </c>
-      <c r="AA23" t="n">
+      <c r="AB23" t="n">
         <v>104429</v>
       </c>
-      <c r="AB23" t="n">
+      <c r="AC23" t="n">
         <v>77457</v>
       </c>
-      <c r="AC23" t="n">
+      <c r="AD23" t="n">
         <v>63355</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>cash dividends declared per share</t>
+          <t>Cash dividends declared per share</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.57</v>
+        <v>2.18</v>
       </c>
       <c r="C24" t="n">
         <v>0.57</v>
       </c>
       <c r="D24" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="E24" t="n">
         <v>0.63</v>
       </c>
-      <c r="E24" t="n">
+      <c r="F24" t="n">
         <v>1.77</v>
       </c>
-      <c r="F24" t="n">
+      <c r="G24" t="n">
         <v>2.4</v>
-      </c>
-      <c r="G24" t="n">
-        <v>0.63</v>
       </c>
       <c r="H24" t="n">
         <v>0.63</v>
       </c>
       <c r="I24" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="J24" t="n">
         <v>0.73</v>
       </c>
-      <c r="J24" t="n">
+      <c r="K24" t="n">
         <v>-0.73</v>
       </c>
-      <c r="K24" t="inlineStr"/>
       <c r="L24" t="inlineStr"/>
       <c r="M24" t="inlineStr"/>
       <c r="N24" t="inlineStr"/>
@@ -2295,11 +2354,12 @@
       <c r="AA24" t="inlineStr"/>
       <c r="AB24" t="inlineStr"/>
       <c r="AC24" t="inlineStr"/>
+      <c r="AD24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>cost of sales</t>
+          <t>Cost of sales</t>
         </is>
       </c>
       <c r="B25" t="inlineStr"/>
@@ -2312,65 +2372,66 @@
       <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr"/>
-      <c r="L25" t="n">
+      <c r="L25" t="inlineStr"/>
+      <c r="M25" t="n">
         <v>48238</v>
       </c>
-      <c r="M25" t="n">
+      <c r="N25" t="n">
         <v>32047</v>
       </c>
-      <c r="N25" t="n">
+      <c r="O25" t="n">
         <v>29473</v>
       </c>
-      <c r="O25" t="n">
+      <c r="P25" t="n">
         <v>115523</v>
       </c>
-      <c r="P25" t="n">
+      <c r="Q25" t="n">
         <v>144996</v>
       </c>
-      <c r="Q25" t="n">
+      <c r="R25" t="n">
         <v>52075</v>
       </c>
-      <c r="R25" t="n">
+      <c r="S25" t="n">
         <v>31321</v>
       </c>
-      <c r="S25" t="n">
+      <c r="T25" t="n">
         <v>32693</v>
       </c>
-      <c r="T25" t="n">
+      <c r="U25" t="n">
         <v>118593</v>
       </c>
-      <c r="U25" t="n">
+      <c r="V25" t="n">
         <v>151286</v>
       </c>
-      <c r="V25" t="n">
+      <c r="W25" t="n">
         <v>62130</v>
       </c>
-      <c r="W25" t="n">
+      <c r="X25" t="n">
         <v>46447</v>
       </c>
-      <c r="X25" t="n">
+      <c r="Y25" t="n">
         <v>40899</v>
       </c>
-      <c r="Y25" t="n">
+      <c r="Z25" t="n">
         <v>151367</v>
       </c>
-      <c r="Z25" t="n">
+      <c r="AA25" t="n">
         <v>192266</v>
       </c>
-      <c r="AA25" t="n">
+      <c r="AB25" t="n">
         <v>64309</v>
       </c>
-      <c r="AB25" t="n">
+      <c r="AC25" t="n">
         <v>49290</v>
       </c>
-      <c r="AC25" t="n">
+      <c r="AD25" t="n">
         <v>41485</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>services</t>
+          <t>Services</t>
         </is>
       </c>
       <c r="B26" t="inlineStr"/>
@@ -2400,7 +2461,8 @@
       <c r="Z26" t="inlineStr"/>
       <c r="AA26" t="inlineStr"/>
       <c r="AB26" t="inlineStr"/>
-      <c r="AC26" t="inlineStr">
+      <c r="AC26" t="inlineStr"/>
+      <c r="AD26" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -2409,7 +2471,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>net sales</t>
+          <t>Net sales</t>
         </is>
       </c>
       <c r="B27" t="inlineStr"/>
@@ -2422,65 +2484,66 @@
       <c r="I27" t="inlineStr"/>
       <c r="J27" t="inlineStr"/>
       <c r="K27" t="inlineStr"/>
-      <c r="L27" t="n">
+      <c r="L27" t="inlineStr"/>
+      <c r="M27" t="n">
         <v>10875</v>
       </c>
-      <c r="M27" t="n">
+      <c r="N27" t="n">
         <v>11450</v>
       </c>
-      <c r="N27" t="n">
+      <c r="O27" t="n">
         <v>11455</v>
       </c>
-      <c r="O27" t="n">
+      <c r="P27" t="n">
         <v>34836</v>
       </c>
-      <c r="P27" t="n">
+      <c r="Q27" t="n">
         <v>46291</v>
       </c>
-      <c r="Q27" t="n">
+      <c r="R27" t="n">
         <v>12715</v>
       </c>
-      <c r="R27" t="n">
+      <c r="S27" t="n">
         <v>13348</v>
       </c>
-      <c r="S27" t="n">
+      <c r="T27" t="n">
         <v>13156</v>
       </c>
-      <c r="T27" t="n">
+      <c r="U27" t="n">
         <v>40612</v>
       </c>
-      <c r="U27" t="n">
+      <c r="V27" t="n">
         <v>53768</v>
       </c>
-      <c r="V27" t="n">
+      <c r="W27" t="n">
         <v>15761</v>
       </c>
-      <c r="W27" t="n">
+      <c r="X27" t="n">
         <v>16901</v>
       </c>
-      <c r="X27" t="n">
+      <c r="Y27" t="n">
         <v>17486</v>
       </c>
-      <c r="Y27" t="n">
+      <c r="Z27" t="n">
         <v>50939</v>
       </c>
-      <c r="Z27" t="n">
+      <c r="AA27" t="n">
         <v>68425</v>
       </c>
-      <c r="AA27" t="n">
+      <c r="AB27" t="n">
         <v>19516</v>
       </c>
-      <c r="AB27" t="n">
+      <c r="AC27" t="n">
         <v>19821</v>
       </c>
-      <c r="AC27" t="n">
+      <c r="AD27" t="n">
         <v>19604</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>cost of sales</t>
+          <t>Cost of sales</t>
         </is>
       </c>
       <c r="B28" t="inlineStr"/>
@@ -2493,58 +2556,59 @@
       <c r="I28" t="inlineStr"/>
       <c r="J28" t="inlineStr"/>
       <c r="K28" t="inlineStr"/>
-      <c r="L28" t="n">
+      <c r="L28" t="inlineStr"/>
+      <c r="M28" t="n">
         <v>4041</v>
       </c>
-      <c r="M28" t="n">
+      <c r="N28" t="n">
         <v>4147</v>
       </c>
-      <c r="N28" t="n">
+      <c r="O28" t="n">
         <v>4109</v>
       </c>
-      <c r="O28" t="n">
+      <c r="P28" t="n">
         <v>12677</v>
       </c>
-      <c r="P28" t="n">
+      <c r="Q28" t="n">
         <v>16786</v>
       </c>
-      <c r="Q28" t="n">
+      <c r="R28" t="n">
         <v>4527</v>
       </c>
-      <c r="R28" t="n">
+      <c r="S28" t="n">
         <v>4622</v>
       </c>
-      <c r="S28" t="n">
+      <c r="T28" t="n">
         <v>4312</v>
       </c>
-      <c r="T28" t="n">
+      <c r="U28" t="n">
         <v>13961</v>
       </c>
-      <c r="U28" t="n">
+      <c r="V28" t="n">
         <v>18273</v>
       </c>
-      <c r="V28" t="n">
+      <c r="W28" t="n">
         <v>4981</v>
       </c>
-      <c r="W28" t="n">
+      <c r="X28" t="n">
         <v>5058</v>
       </c>
-      <c r="X28" t="n">
+      <c r="Y28" t="n">
         <v>5280</v>
       </c>
-      <c r="Y28" t="n">
+      <c r="Z28" t="n">
         <v>15435</v>
       </c>
-      <c r="Z28" t="n">
+      <c r="AA28" t="n">
         <v>20715</v>
       </c>
-      <c r="AA28" t="n">
+      <c r="AB28" t="n">
         <v>5393</v>
       </c>
-      <c r="AB28" t="n">
+      <c r="AC28" t="n">
         <v>5429</v>
       </c>
-      <c r="AC28" t="n">
+      <c r="AD28" t="n">
         <v>5589</v>
       </c>
     </row>
@@ -2742,7 +2806,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>income statement [abstract]</t>
+          <t>Income statement [abstract]</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -2752,7 +2816,7 @@
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
         <is>
-          <t>income statement [abstract]</t>
+          <t>Income statement [abstract]</t>
         </is>
       </c>
       <c r="H2" t="inlineStr"/>
@@ -2762,7 +2826,7 @@
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr">
         <is>
-          <t>net sales</t>
+          <t>Net sales</t>
         </is>
       </c>
       <c r="N2" t="n">
@@ -2782,7 +2846,7 @@
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>net sales</t>
+          <t>Net sales</t>
         </is>
       </c>
       <c r="T2" t="n">
@@ -2802,7 +2866,7 @@
       </c>
       <c r="Y2" t="inlineStr">
         <is>
-          <t>net sales</t>
+          <t>Net sales</t>
         </is>
       </c>
       <c r="Z2" t="n">
@@ -2822,7 +2886,7 @@
       </c>
       <c r="AE2" t="inlineStr">
         <is>
-          <t>net sales</t>
+          <t>Net sales</t>
         </is>
       </c>
       <c r="AF2" t="n">
@@ -2838,7 +2902,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>net sales</t>
+          <t>Net sales</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -2858,7 +2922,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>net sales</t>
+          <t>Net sales</t>
         </is>
       </c>
       <c r="H3" t="n">
@@ -2878,7 +2942,7 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>cost of sales</t>
+          <t>Cost of sales</t>
         </is>
       </c>
       <c r="N3" t="n">
@@ -2898,7 +2962,7 @@
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>cost of sales</t>
+          <t>Cost of sales</t>
         </is>
       </c>
       <c r="T3" t="n">
@@ -2918,7 +2982,7 @@
       </c>
       <c r="Y3" t="inlineStr">
         <is>
-          <t>cost of sales</t>
+          <t>Cost of sales</t>
         </is>
       </c>
       <c r="Z3" t="n">
@@ -2938,7 +3002,7 @@
       </c>
       <c r="AE3" t="inlineStr">
         <is>
-          <t>cost of sales</t>
+          <t>Cost of sales</t>
         </is>
       </c>
       <c r="AF3" t="n">
@@ -2954,7 +3018,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>cost of sales</t>
+          <t>Cost of sales</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -2974,7 +3038,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>cost of sales</t>
+          <t>Cost of sales</t>
         </is>
       </c>
       <c r="H4" t="n">
@@ -2994,7 +3058,7 @@
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>gross margin</t>
+          <t>Gross margin</t>
         </is>
       </c>
       <c r="N4" t="n">
@@ -3014,7 +3078,7 @@
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>gross margin</t>
+          <t>Gross margin</t>
         </is>
       </c>
       <c r="T4" t="n">
@@ -3034,7 +3098,7 @@
       </c>
       <c r="Y4" t="inlineStr">
         <is>
-          <t>gross margin</t>
+          <t>Gross margin</t>
         </is>
       </c>
       <c r="Z4" t="n">
@@ -3054,7 +3118,7 @@
       </c>
       <c r="AE4" t="inlineStr">
         <is>
-          <t>gross margin</t>
+          <t>Gross margin</t>
         </is>
       </c>
       <c r="AF4" t="n">
@@ -3070,7 +3134,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>gross margin</t>
+          <t>Gross margin</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -3090,7 +3154,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>gross margin</t>
+          <t>Gross margin</t>
         </is>
       </c>
       <c r="H5" t="n">
@@ -3110,7 +3174,7 @@
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>operating expenses:</t>
+          <t>Operating expenses:</t>
         </is>
       </c>
       <c r="N5" t="inlineStr"/>
@@ -3120,7 +3184,7 @@
       <c r="R5" t="inlineStr"/>
       <c r="S5" t="inlineStr">
         <is>
-          <t>operating expenses:</t>
+          <t>Operating expenses:</t>
         </is>
       </c>
       <c r="T5" t="inlineStr"/>
@@ -3130,7 +3194,7 @@
       <c r="X5" t="inlineStr"/>
       <c r="Y5" t="inlineStr">
         <is>
-          <t>operating expenses:</t>
+          <t>Operating expenses:</t>
         </is>
       </c>
       <c r="Z5" t="inlineStr"/>
@@ -3140,7 +3204,7 @@
       <c r="AD5" t="inlineStr"/>
       <c r="AE5" t="inlineStr">
         <is>
-          <t>operating expenses:</t>
+          <t>Operating expenses:</t>
         </is>
       </c>
       <c r="AF5" t="inlineStr"/>
@@ -3154,7 +3218,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>operating expenses:</t>
+          <t>Operating expenses:</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
@@ -3164,7 +3228,7 @@
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr">
         <is>
-          <t>operating expenses:</t>
+          <t>Operating expenses:</t>
         </is>
       </c>
       <c r="H6" t="inlineStr"/>
@@ -3174,7 +3238,7 @@
       <c r="L6" t="inlineStr"/>
       <c r="M6" t="inlineStr">
         <is>
-          <t>research and development</t>
+          <t>Research and development</t>
         </is>
       </c>
       <c r="N6" t="n">
@@ -3194,7 +3258,7 @@
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>research and development</t>
+          <t>Research and development</t>
         </is>
       </c>
       <c r="T6" t="n">
@@ -3214,7 +3278,7 @@
       </c>
       <c r="Y6" t="inlineStr">
         <is>
-          <t>research and development</t>
+          <t>Research and development</t>
         </is>
       </c>
       <c r="Z6" t="n">
@@ -3234,7 +3298,7 @@
       </c>
       <c r="AE6" t="inlineStr">
         <is>
-          <t>research and development</t>
+          <t>Research and development</t>
         </is>
       </c>
       <c r="AF6" t="n">
@@ -3250,7 +3314,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>research and development</t>
+          <t>Research and development</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -3270,7 +3334,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>research and development</t>
+          <t>Research and development</t>
         </is>
       </c>
       <c r="H7" t="n">
@@ -3290,7 +3354,7 @@
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>selling, general and administrative</t>
+          <t>Selling, general and administrative</t>
         </is>
       </c>
       <c r="N7" t="n">
@@ -3310,7 +3374,7 @@
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>selling, general and administrative</t>
+          <t>Selling, general and administrative</t>
         </is>
       </c>
       <c r="T7" t="n">
@@ -3330,7 +3394,7 @@
       </c>
       <c r="Y7" t="inlineStr">
         <is>
-          <t>selling, general and administrative</t>
+          <t>Selling, general and administrative</t>
         </is>
       </c>
       <c r="Z7" t="n">
@@ -3350,7 +3414,7 @@
       </c>
       <c r="AE7" t="inlineStr">
         <is>
-          <t>selling, general and administrative</t>
+          <t>Selling, general and administrative</t>
         </is>
       </c>
       <c r="AF7" t="n">
@@ -3366,7 +3430,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>selling, general and administrative</t>
+          <t>Selling, general and administrative</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -3386,7 +3450,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>selling, general and administrative</t>
+          <t>Selling, general and administrative</t>
         </is>
       </c>
       <c r="H8" t="n">
@@ -3406,7 +3470,7 @@
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>total operating expenses</t>
+          <t>Total operating expenses</t>
         </is>
       </c>
       <c r="N8" t="n">
@@ -3426,7 +3490,7 @@
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>total operating expenses</t>
+          <t>Total operating expenses</t>
         </is>
       </c>
       <c r="T8" t="n">
@@ -3446,7 +3510,7 @@
       </c>
       <c r="Y8" t="inlineStr">
         <is>
-          <t>total operating expenses</t>
+          <t>Total operating expenses</t>
         </is>
       </c>
       <c r="Z8" t="n">
@@ -3466,7 +3530,7 @@
       </c>
       <c r="AE8" t="inlineStr">
         <is>
-          <t>total operating expenses</t>
+          <t>Total operating expenses</t>
         </is>
       </c>
       <c r="AF8" t="n">
@@ -3482,7 +3546,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>total operating expenses</t>
+          <t>Total operating expenses</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -3502,7 +3566,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>total operating expenses</t>
+          <t>Total operating expenses</t>
         </is>
       </c>
       <c r="H9" t="n">
@@ -3522,7 +3586,7 @@
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>operating income</t>
+          <t>Operating income</t>
         </is>
       </c>
       <c r="N9" t="n">
@@ -3542,7 +3606,7 @@
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>operating income</t>
+          <t>Operating income</t>
         </is>
       </c>
       <c r="T9" t="n">
@@ -3562,7 +3626,7 @@
       </c>
       <c r="Y9" t="inlineStr">
         <is>
-          <t>operating income</t>
+          <t>Operating income</t>
         </is>
       </c>
       <c r="Z9" t="n">
@@ -3582,7 +3646,7 @@
       </c>
       <c r="AE9" t="inlineStr">
         <is>
-          <t>operating income</t>
+          <t>Operating income</t>
         </is>
       </c>
       <c r="AF9" t="n">
@@ -3598,7 +3662,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>operating income</t>
+          <t>Operating income</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -3618,7 +3682,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>operating income</t>
+          <t>Operating income</t>
         </is>
       </c>
       <c r="H10" t="n">
@@ -3638,7 +3702,7 @@
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>other income, net</t>
+          <t>Other income/, net</t>
         </is>
       </c>
       <c r="N10" t="n">
@@ -3658,7 +3722,7 @@
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>other income, net</t>
+          <t>Other income/, net</t>
         </is>
       </c>
       <c r="T10" t="n">
@@ -3678,7 +3742,7 @@
       </c>
       <c r="Y10" t="inlineStr">
         <is>
-          <t>other income, net</t>
+          <t>Other income/, net</t>
         </is>
       </c>
       <c r="Z10" t="n">
@@ -3698,7 +3762,7 @@
       </c>
       <c r="AE10" t="inlineStr">
         <is>
-          <t>other income, net</t>
+          <t>Other income/, net</t>
         </is>
       </c>
       <c r="AF10" t="n">
@@ -3714,7 +3778,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>other income, net</t>
+          <t>Other income/, net</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -3734,7 +3798,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>other income, net</t>
+          <t>Other income/, net</t>
         </is>
       </c>
       <c r="H11" t="n">
@@ -3754,7 +3818,7 @@
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>income before provision for income taxes</t>
+          <t>Income before provision for income taxes</t>
         </is>
       </c>
       <c r="N11" t="n">
@@ -3774,7 +3838,7 @@
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>income before provision for income taxes</t>
+          <t>Income before provision for income taxes</t>
         </is>
       </c>
       <c r="T11" t="n">
@@ -3794,7 +3858,7 @@
       </c>
       <c r="Y11" t="inlineStr">
         <is>
-          <t>income before provision for income taxes</t>
+          <t>Income before provision for income taxes</t>
         </is>
       </c>
       <c r="Z11" t="n">
@@ -3814,7 +3878,7 @@
       </c>
       <c r="AE11" t="inlineStr">
         <is>
-          <t>income before provision for income taxes</t>
+          <t>Income before provision for income taxes</t>
         </is>
       </c>
       <c r="AF11" t="n">
@@ -3830,7 +3894,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>income before provision for income taxes</t>
+          <t>Income before provision for income taxes</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -3850,7 +3914,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>income before provision for income taxes</t>
+          <t>Income before provision for income taxes</t>
         </is>
       </c>
       <c r="H12" t="n">
@@ -3870,7 +3934,7 @@
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>provision for income taxes</t>
+          <t>Provision for income taxes</t>
         </is>
       </c>
       <c r="N12" t="n">
@@ -3890,7 +3954,7 @@
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>provision for income taxes</t>
+          <t>Provision for income taxes</t>
         </is>
       </c>
       <c r="T12" t="n">
@@ -3910,7 +3974,7 @@
       </c>
       <c r="Y12" t="inlineStr">
         <is>
-          <t>provision for income taxes</t>
+          <t>Provision for income taxes</t>
         </is>
       </c>
       <c r="Z12" t="n">
@@ -3930,7 +3994,7 @@
       </c>
       <c r="AE12" t="inlineStr">
         <is>
-          <t>provision for income taxes</t>
+          <t>Provision for income taxes</t>
         </is>
       </c>
       <c r="AF12" t="n">
@@ -3946,7 +4010,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>provision for income taxes</t>
+          <t>Provision for income taxes</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -3966,7 +4030,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>provision for income taxes</t>
+          <t>Provision for income taxes</t>
         </is>
       </c>
       <c r="H13" t="n">
@@ -3986,7 +4050,7 @@
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>net income</t>
+          <t>Net income</t>
         </is>
       </c>
       <c r="N13" t="n">
@@ -4006,7 +4070,7 @@
       </c>
       <c r="S13" t="inlineStr">
         <is>
-          <t>net income</t>
+          <t>Net income</t>
         </is>
       </c>
       <c r="T13" t="n">
@@ -4026,7 +4090,7 @@
       </c>
       <c r="Y13" t="inlineStr">
         <is>
-          <t>net income</t>
+          <t>Net income</t>
         </is>
       </c>
       <c r="Z13" t="n">
@@ -4046,7 +4110,7 @@
       </c>
       <c r="AE13" t="inlineStr">
         <is>
-          <t>net income</t>
+          <t>Net income</t>
         </is>
       </c>
       <c r="AF13" t="n">
@@ -4062,7 +4126,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>net income</t>
+          <t>Net income</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -4082,7 +4146,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>net income</t>
+          <t>Net income</t>
         </is>
       </c>
       <c r="H14" t="n">
@@ -4102,7 +4166,7 @@
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>earnings per share:</t>
+          <t>Earnings per share:</t>
         </is>
       </c>
       <c r="N14" t="inlineStr"/>
@@ -4112,7 +4176,7 @@
       <c r="R14" t="inlineStr"/>
       <c r="S14" t="inlineStr">
         <is>
-          <t>earnings per share:</t>
+          <t>Earnings per share:</t>
         </is>
       </c>
       <c r="T14" t="inlineStr"/>
@@ -4122,7 +4186,7 @@
       <c r="X14" t="inlineStr"/>
       <c r="Y14" t="inlineStr">
         <is>
-          <t>earnings per share:</t>
+          <t>Earnings per share:</t>
         </is>
       </c>
       <c r="Z14" t="inlineStr"/>
@@ -4132,7 +4196,7 @@
       <c r="AD14" t="inlineStr"/>
       <c r="AE14" t="inlineStr">
         <is>
-          <t>earnings per share [abstract]</t>
+          <t>Earnings per share [abstract]</t>
         </is>
       </c>
       <c r="AF14" t="inlineStr"/>
@@ -4142,7 +4206,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>earnings per share:</t>
+          <t>Earnings per share:</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
@@ -4152,7 +4216,7 @@
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr">
         <is>
-          <t>earnings per share:</t>
+          <t>Earnings per share:</t>
         </is>
       </c>
       <c r="H15" t="inlineStr"/>
@@ -4162,7 +4226,7 @@
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="inlineStr">
         <is>
-          <t>basic</t>
+          <t>Basic</t>
         </is>
       </c>
       <c r="N15" t="n">
@@ -4182,7 +4246,7 @@
       </c>
       <c r="S15" t="inlineStr">
         <is>
-          <t>basic</t>
+          <t>Basic</t>
         </is>
       </c>
       <c r="T15" t="n">
@@ -4202,7 +4266,7 @@
       </c>
       <c r="Y15" t="inlineStr">
         <is>
-          <t>basic</t>
+          <t>Basic</t>
         </is>
       </c>
       <c r="Z15" t="n">
@@ -4222,7 +4286,7 @@
       </c>
       <c r="AE15" t="inlineStr">
         <is>
-          <t>earnings per share:</t>
+          <t>Earnings per share:</t>
         </is>
       </c>
       <c r="AF15" t="inlineStr"/>
@@ -4236,7 +4300,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>basic</t>
+          <t>Basic</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -4256,7 +4320,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>basic</t>
+          <t>Basic</t>
         </is>
       </c>
       <c r="H16" t="n">
@@ -4276,7 +4340,7 @@
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>diluted</t>
+          <t>Diluted</t>
         </is>
       </c>
       <c r="N16" t="n">
@@ -4296,7 +4360,7 @@
       </c>
       <c r="S16" t="inlineStr">
         <is>
-          <t>diluted</t>
+          <t>Diluted</t>
         </is>
       </c>
       <c r="T16" t="n">
@@ -4316,7 +4380,7 @@
       </c>
       <c r="Y16" t="inlineStr">
         <is>
-          <t>diluted</t>
+          <t>Diluted</t>
         </is>
       </c>
       <c r="Z16" t="n">
@@ -4336,7 +4400,7 @@
       </c>
       <c r="AE16" t="inlineStr">
         <is>
-          <t>basic</t>
+          <t>Basic</t>
         </is>
       </c>
       <c r="AF16" t="n">
@@ -4352,7 +4416,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>diluted</t>
+          <t>Diluted</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -4372,7 +4436,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>diluted</t>
+          <t>Diluted</t>
         </is>
       </c>
       <c r="H17" t="n">
@@ -4392,7 +4456,7 @@
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>shares used in computing earnings per share:</t>
+          <t>Shares used in computing earnings per share:</t>
         </is>
       </c>
       <c r="N17" t="inlineStr"/>
@@ -4402,7 +4466,7 @@
       <c r="R17" t="inlineStr"/>
       <c r="S17" t="inlineStr">
         <is>
-          <t>shares used in computing earnings per share:</t>
+          <t>Shares used in computing earnings per share:</t>
         </is>
       </c>
       <c r="T17" t="inlineStr"/>
@@ -4412,7 +4476,7 @@
       <c r="X17" t="inlineStr"/>
       <c r="Y17" t="inlineStr">
         <is>
-          <t>shares used in computing earnings per share:</t>
+          <t>Shares used in computing earnings per share:</t>
         </is>
       </c>
       <c r="Z17" t="inlineStr"/>
@@ -4422,7 +4486,7 @@
       <c r="AD17" t="inlineStr"/>
       <c r="AE17" t="inlineStr">
         <is>
-          <t>diluted</t>
+          <t>Diluted</t>
         </is>
       </c>
       <c r="AF17" t="n">
@@ -4438,7 +4502,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>shares used in computing earnings per share:</t>
+          <t>Shares used in computing earnings per share:</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
@@ -4448,7 +4512,7 @@
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr">
         <is>
-          <t>shares used in computing earnings per share:</t>
+          <t>Shares used in computing earnings per share:</t>
         </is>
       </c>
       <c r="H18" t="inlineStr"/>
@@ -4458,7 +4522,7 @@
       <c r="L18" t="inlineStr"/>
       <c r="M18" t="inlineStr">
         <is>
-          <t>basic</t>
+          <t>Basic</t>
         </is>
       </c>
       <c r="N18" t="n">
@@ -4478,7 +4542,7 @@
       </c>
       <c r="S18" t="inlineStr">
         <is>
-          <t>basic</t>
+          <t>Basic</t>
         </is>
       </c>
       <c r="T18" t="n">
@@ -4498,7 +4562,7 @@
       </c>
       <c r="Y18" t="inlineStr">
         <is>
-          <t>basic</t>
+          <t>Basic</t>
         </is>
       </c>
       <c r="Z18" t="n">
@@ -4518,7 +4582,7 @@
       </c>
       <c r="AE18" t="inlineStr">
         <is>
-          <t>shares used in computing earnings per share:</t>
+          <t>Shares used in computing earnings per share:</t>
         </is>
       </c>
       <c r="AF18" t="inlineStr"/>
@@ -4532,7 +4596,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>basic</t>
+          <t>Basic</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -4552,7 +4616,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>basic</t>
+          <t>Basic</t>
         </is>
       </c>
       <c r="H19" t="n">
@@ -4572,7 +4636,7 @@
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>diluted</t>
+          <t>Diluted</t>
         </is>
       </c>
       <c r="N19" t="n">
@@ -4592,7 +4656,7 @@
       </c>
       <c r="S19" t="inlineStr">
         <is>
-          <t>diluted</t>
+          <t>Diluted</t>
         </is>
       </c>
       <c r="T19" t="n">
@@ -4612,7 +4676,7 @@
       </c>
       <c r="Y19" t="inlineStr">
         <is>
-          <t>diluted</t>
+          <t>Diluted</t>
         </is>
       </c>
       <c r="Z19" t="n">
@@ -4632,7 +4696,7 @@
       </c>
       <c r="AE19" t="inlineStr">
         <is>
-          <t>basic</t>
+          <t>Basic</t>
         </is>
       </c>
       <c r="AF19" t="n">
@@ -4648,7 +4712,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>diluted</t>
+          <t>Diluted</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -4668,7 +4732,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>diluted</t>
+          <t>Diluted</t>
         </is>
       </c>
       <c r="H20" t="n">
@@ -4688,7 +4752,7 @@
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>products</t>
+          <t>Products</t>
         </is>
       </c>
       <c r="N20" t="inlineStr"/>
@@ -4698,7 +4762,7 @@
       <c r="R20" t="inlineStr"/>
       <c r="S20" t="inlineStr">
         <is>
-          <t>products</t>
+          <t>Products</t>
         </is>
       </c>
       <c r="T20" t="inlineStr"/>
@@ -4708,7 +4772,7 @@
       <c r="X20" t="inlineStr"/>
       <c r="Y20" t="inlineStr">
         <is>
-          <t>products</t>
+          <t>Products</t>
         </is>
       </c>
       <c r="Z20" t="inlineStr"/>
@@ -4718,7 +4782,7 @@
       <c r="AD20" t="inlineStr"/>
       <c r="AE20" t="inlineStr">
         <is>
-          <t>diluted</t>
+          <t>Diluted</t>
         </is>
       </c>
       <c r="AF20" t="n">
@@ -4734,7 +4798,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>cash dividends declared per share</t>
+          <t>Cash dividends declared per share</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -4754,7 +4818,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>cash dividends declared per share</t>
+          <t>Cash dividends declared per share</t>
         </is>
       </c>
       <c r="H21" t="n">
@@ -4772,7 +4836,7 @@
       <c r="L21" t="inlineStr"/>
       <c r="M21" t="inlineStr">
         <is>
-          <t>net sales</t>
+          <t>Net sales</t>
         </is>
       </c>
       <c r="N21" t="n">
@@ -4792,7 +4856,7 @@
       </c>
       <c r="S21" t="inlineStr">
         <is>
-          <t>net sales</t>
+          <t>Net sales</t>
         </is>
       </c>
       <c r="T21" t="n">
@@ -4812,7 +4876,7 @@
       </c>
       <c r="Y21" t="inlineStr">
         <is>
-          <t>net sales</t>
+          <t>Net sales</t>
         </is>
       </c>
       <c r="Z21" t="n">
@@ -4832,7 +4896,7 @@
       </c>
       <c r="AE21" t="inlineStr">
         <is>
-          <t>products</t>
+          <t>Products</t>
         </is>
       </c>
       <c r="AF21" t="inlineStr"/>
@@ -4858,7 +4922,7 @@
       <c r="L22" t="inlineStr"/>
       <c r="M22" t="inlineStr">
         <is>
-          <t>cost of sales</t>
+          <t>Cost of sales</t>
         </is>
       </c>
       <c r="N22" t="n">
@@ -4878,7 +4942,7 @@
       </c>
       <c r="S22" t="inlineStr">
         <is>
-          <t>cost of sales</t>
+          <t>Cost of sales</t>
         </is>
       </c>
       <c r="T22" t="n">
@@ -4898,7 +4962,7 @@
       </c>
       <c r="Y22" t="inlineStr">
         <is>
-          <t>cost of sales</t>
+          <t>Cost of sales</t>
         </is>
       </c>
       <c r="Z22" t="n">
@@ -4918,7 +4982,7 @@
       </c>
       <c r="AE22" t="inlineStr">
         <is>
-          <t>net sales</t>
+          <t>Net sales</t>
         </is>
       </c>
       <c r="AF22" t="n">
@@ -4946,7 +5010,7 @@
       <c r="L23" t="inlineStr"/>
       <c r="M23" t="inlineStr">
         <is>
-          <t>services</t>
+          <t>Services</t>
         </is>
       </c>
       <c r="N23" t="inlineStr"/>
@@ -4956,7 +5020,7 @@
       <c r="R23" t="inlineStr"/>
       <c r="S23" t="inlineStr">
         <is>
-          <t>services</t>
+          <t>Services</t>
         </is>
       </c>
       <c r="T23" t="inlineStr"/>
@@ -4966,7 +5030,7 @@
       <c r="X23" t="inlineStr"/>
       <c r="Y23" t="inlineStr">
         <is>
-          <t>services</t>
+          <t>Services</t>
         </is>
       </c>
       <c r="Z23" t="inlineStr"/>
@@ -4976,7 +5040,7 @@
       <c r="AD23" t="inlineStr"/>
       <c r="AE23" t="inlineStr">
         <is>
-          <t>cost of sales</t>
+          <t>Cost of sales</t>
         </is>
       </c>
       <c r="AF23" t="n">
@@ -5004,7 +5068,7 @@
       <c r="L24" t="inlineStr"/>
       <c r="M24" t="inlineStr">
         <is>
-          <t>net sales</t>
+          <t>Net sales</t>
         </is>
       </c>
       <c r="N24" t="n">
@@ -5024,7 +5088,7 @@
       </c>
       <c r="S24" t="inlineStr">
         <is>
-          <t>net sales</t>
+          <t>Net sales</t>
         </is>
       </c>
       <c r="T24" t="n">
@@ -5044,7 +5108,7 @@
       </c>
       <c r="Y24" t="inlineStr">
         <is>
-          <t>net sales</t>
+          <t>Net sales</t>
         </is>
       </c>
       <c r="Z24" t="n">
@@ -5064,7 +5128,7 @@
       </c>
       <c r="AE24" t="inlineStr">
         <is>
-          <t>services</t>
+          <t>Services</t>
         </is>
       </c>
       <c r="AF24" t="inlineStr"/>
@@ -5090,7 +5154,7 @@
       <c r="L25" t="inlineStr"/>
       <c r="M25" t="inlineStr">
         <is>
-          <t>cost of sales</t>
+          <t>Cost of sales</t>
         </is>
       </c>
       <c r="N25" t="n">
@@ -5110,7 +5174,7 @@
       </c>
       <c r="S25" t="inlineStr">
         <is>
-          <t>cost of sales</t>
+          <t>Cost of sales</t>
         </is>
       </c>
       <c r="T25" t="n">
@@ -5130,7 +5194,7 @@
       </c>
       <c r="Y25" t="inlineStr">
         <is>
-          <t>cost of sales</t>
+          <t>Cost of sales</t>
         </is>
       </c>
       <c r="Z25" t="n">
@@ -5150,7 +5214,7 @@
       </c>
       <c r="AE25" t="inlineStr">
         <is>
-          <t>net sales</t>
+          <t>Net sales</t>
         </is>
       </c>
       <c r="AF25" t="n">
@@ -5196,7 +5260,7 @@
       <c r="AD26" t="inlineStr"/>
       <c r="AE26" t="inlineStr">
         <is>
-          <t>cost of sales</t>
+          <t>Cost of sales</t>
         </is>
       </c>
       <c r="AF26" t="n">

</xml_diff>